<commit_message>
add ground_warfae files and data
.
</commit_message>
<xml_diff>
--- a/Data/Test/dataset1/input_data.xlsx
+++ b/Data/Test/dataset1/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sueng\PycharmProjects\AI_SH_graph_rev_rev1\Data\Test\dataset1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e18d0fa5f3bb7c54/AISH2/AISH/Data/Test/dataset1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6FBF88-96F5-4024-BC38-2582DC338A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{AA6FBF88-96F5-4024-BC38-2582DC338A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{138CE40D-F6CC-40FA-8453-F9A54E28CB45}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="3120" windowWidth="13320" windowHeight="9450" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ship" sheetId="1" r:id="rId1"/>
@@ -549,13 +549,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -589,7 +589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -606,7 +606,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -623,7 +623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -640,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -657,24 +657,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -691,7 +691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -708,24 +708,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>12</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -742,12 +742,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>20</v>
@@ -759,7 +759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -770,30 +770,30 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -810,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -827,7 +827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -844,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -861,7 +861,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -878,7 +878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -912,7 +912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -929,7 +929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -946,24 +946,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D24">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="E24">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -980,7 +980,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -997,7 +997,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1116,41 +1116,41 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1212,12 +1212,12 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1231,21 +1231,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
       <c r="C2">
-        <v>1.4</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1315,21 +1315,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="C8">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="D8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1452,12 +1452,12 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E16"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1474,41 +1474,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="D2">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="E2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1743,9 +1743,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1833,15 +1833,15 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1849,15 +1849,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
       <c r="B2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>

</xml_diff>